<commit_message>
Definiciones agregadas al diccionario de datos
</commit_message>
<xml_diff>
--- a/diccionario de datos.xlsx
+++ b/diccionario de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias Actis Grosso\Documents\Elias\Personal\Capacitación\Data\Data Science - Coder\TP final\ds-ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F221B82C-3566-4D52-92BB-936B2E33BEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA00EA12-44A8-40C1-8D6A-CFAC19208CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>ecomm_order_id</t>
   </si>
@@ -130,6 +130,72 @@
   </si>
   <si>
     <t>Descripción</t>
+  </si>
+  <si>
+    <t>Precio que pagó el cliente por el artículo</t>
+  </si>
+  <si>
+    <t>Costo del producto para la empresa</t>
+  </si>
+  <si>
+    <t>Valor de venta sin promociones ni descuentos</t>
+  </si>
+  <si>
+    <t>Costo del producto para la empresa (debería ser igual a PrecioCosto)</t>
+  </si>
+  <si>
+    <t>Tienda en la que se realizó la compra</t>
+  </si>
+  <si>
+    <t>ecommerce a través del cual se realizó la compra</t>
+  </si>
+  <si>
+    <t>ID de orden de compra</t>
+  </si>
+  <si>
+    <t>Fecha y hora de la transacción</t>
+  </si>
+  <si>
+    <t>Categoría del artículo comprado</t>
+  </si>
+  <si>
+    <t>Marca del artículo comprado</t>
+  </si>
+  <si>
+    <t>ID del artículo</t>
+  </si>
+  <si>
+    <t>Talle del artículo</t>
+  </si>
+  <si>
+    <t>Nombre del artículo</t>
+  </si>
+  <si>
+    <t>Cantidad comprada</t>
+  </si>
+  <si>
+    <t>Forma de envío</t>
+  </si>
+  <si>
+    <t>Color del artículo</t>
+  </si>
+  <si>
+    <t>Género del artículo</t>
+  </si>
+  <si>
+    <t>Temática del artículo</t>
+  </si>
+  <si>
+    <t>Método de pago</t>
+  </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>email del comprador (encriptado)</t>
   </si>
 </sst>
 </file>
@@ -458,14 +524,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.1796875" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="60.1796875" customWidth="1"/>
     <col min="3" max="3" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -481,21 +547,33 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -511,135 +589,189 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Notebook con análisis completo y diccionario completo
</commit_message>
<xml_diff>
--- a/diccionario de datos.xlsx
+++ b/diccionario de datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elias Actis Grosso\Documents\Elias\Personal\Capacitación\Data\Data Science - Coder\TP final\ds-ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA00EA12-44A8-40C1-8D6A-CFAC19208CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427B2AAD-CA82-43CB-B97E-FF2B582F9EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>ecomm_order_id</t>
   </si>
@@ -196,22 +196,41 @@
   </si>
   <si>
     <t>email del comprador (encriptado)</t>
+  </si>
+  <si>
+    <t>Fecha en la que se facturó</t>
+  </si>
+  <si>
+    <t>Fecha y hora de la transacción (repetido)</t>
+  </si>
+  <si>
+    <t>Fecha de cuando la empresa empieza a trabajar el pedido</t>
+  </si>
+  <si>
+    <t>Id interno de la dirección de entrega</t>
+  </si>
+  <si>
+    <t>Código interno del proveedor</t>
+  </si>
+  <si>
+    <t>Número de lote</t>
+  </si>
+  <si>
+    <t>Descripción del ecommerce</t>
+  </si>
+  <si>
+    <t>Sucursal de donde salió el producto</t>
+  </si>
+  <si>
+    <t>Sucursal a donde se envió el producto por última vez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -239,9 +258,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,10 +554,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -579,11 +597,17 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -682,11 +706,17 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -700,6 +730,9 @@
       <c r="A23" t="s">
         <v>21</v>
       </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -721,21 +754,33 @@
       <c r="A26" t="s">
         <v>24</v>
       </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -748,6 +793,9 @@
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>